<commit_message>
STLs, BOM and some code
</commit_message>
<xml_diff>
--- a/petFeederBOM.xlsx
+++ b/petFeederBOM.xlsx
@@ -1,31 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lampros\Desktop\ELLAK\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lampros\Desktop\dimkakogeo-pet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{64760E97-DB5C-4F63-9BDE-9DE36456D2C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59976522-9A6F-4F60-9A11-85AA83461EF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D6BB9331-6BCE-4812-BF72-CE035F863465}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Raspberry Pi Zero 2 W</t>
   </si>
@@ -36,27 +47,12 @@
     <t>Raspberry Pi Camera Module</t>
   </si>
   <si>
-    <t>Waveshare Stepper Motor HAT</t>
-  </si>
-  <si>
-    <t>2x Stepper Motor 28YBJ-48</t>
-  </si>
-  <si>
-    <t>Ultrasonic Sensor</t>
-  </si>
-  <si>
-    <t>12V Power Supply</t>
-  </si>
-  <si>
     <t>Κόστος</t>
   </si>
   <si>
     <t>Υλικό</t>
   </si>
   <si>
-    <t>Link (Optional)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Κόστος </t>
   </si>
   <si>
@@ -69,18 +65,6 @@
     <t>Raspberry Pi Zero Camera Adapter</t>
   </si>
   <si>
-    <t>https://www.hellasdigital.gr/go-create/raspberry-and-accessories-el/raspberry-pi/stepper-motor-hat-for-raspberry-pi-drives-two-stepper-motors/?sl=en</t>
-  </si>
-  <si>
-    <t>https://www.hellasdigital.gr/electronics/motors-and-drivers/stepper/28byj-48-4-phase-stepper-motor-dc-5v-for-arduino/</t>
-  </si>
-  <si>
-    <t>https://www.hellasdigital.gr/electronics/sensors/ultasonic/hy-srf05-ultrasonic-distance-sensor-module-replace-sr04-module/</t>
-  </si>
-  <si>
-    <t>https://www.pc1.gr/showitem.php?ID=200000199</t>
-  </si>
-  <si>
     <t>https://grobotronics.com/raspberry-pi-zero-v1.3-camera-cable-80mm.html?sl=en</t>
   </si>
   <si>
@@ -88,6 +72,27 @@
   </si>
   <si>
     <t>1kg PLA/PETG</t>
+  </si>
+  <si>
+    <t>https://www.cableworks.gr/ilektronika/motors/servo/mg996r-servo-metal-gear-high-torque-motor-for-arduino/</t>
+  </si>
+  <si>
+    <t>2*Servo mg996r</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HDMI male to mini HDMI Cable </t>
+  </si>
+  <si>
+    <t>power Supply</t>
+  </si>
+  <si>
+    <t>https://www.hellasdigital.gr/go-create/raspberry-and-accessories/power-supplies/5v-3a-adapter-micro-connector-power-supply/</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>mini HDMI to HDMI cable</t>
   </si>
 </sst>
 </file>
@@ -171,9 +176,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -211,7 +216,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -317,7 +322,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -459,7 +464,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -467,27 +472,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75AC0FC5-E85B-4403-9348-A87EAB984DBF}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="53.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -495,7 +500,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C2" s="2">
         <v>20</v>
@@ -506,7 +511,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C3" s="2">
         <v>10</v>
@@ -517,7 +522,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C4" s="2">
         <v>33</v>
@@ -525,10 +530,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C5" s="2">
         <v>2</v>
@@ -536,7 +541,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2">
@@ -545,46 +550,46 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C7" s="2">
-        <v>20</v>
+        <f>6.32*2</f>
+        <v>12.64</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" s="2">
-        <v>5</v>
+        <v>3.35</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C9" s="2">
-        <v>2</v>
+        <v>2.9</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="A10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="2"/>
       <c r="C10" s="2">
-        <v>8</v>
+        <f ca="1">SUM(C2:C11)</f>
+        <v>103.89</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -592,27 +597,14 @@
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2">
-        <f>SUM(C2:C11)</f>
-        <v>120</v>
-      </c>
-    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{2ABAA7BE-02AD-4C08-B92F-07105F20F350}"/>
-    <hyperlink ref="B7" r:id="rId2" xr:uid="{7F948254-E36D-4C5F-8898-5FC3DED066E2}"/>
-    <hyperlink ref="B8" r:id="rId3" xr:uid="{E6EEFFCF-24DA-46B1-9480-F5AA4C06D772}"/>
-    <hyperlink ref="B9" r:id="rId4" xr:uid="{09A3B0BF-0E6F-45D5-B666-C392FA831274}"/>
-    <hyperlink ref="B5" r:id="rId5" xr:uid="{F2159DCD-E171-4453-B3DB-58FBF95A8A76}"/>
-    <hyperlink ref="B4" r:id="rId6" xr:uid="{E0C03882-9A14-4AB4-90BB-2ABBE6C71310}"/>
-    <hyperlink ref="B10" r:id="rId7" xr:uid="{8B4771D5-0226-42AA-A3DF-DBC09875A010}"/>
+    <hyperlink ref="B5" r:id="rId2" xr:uid="{F2159DCD-E171-4453-B3DB-58FBF95A8A76}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{E0C03882-9A14-4AB4-90BB-2ABBE6C71310}"/>
+    <hyperlink ref="B7" r:id="rId4" xr:uid="{DFD7BC76-8F81-4227-B65F-88F0E4AFA78D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>